<commit_message>
Working on digital filter vignette
</commit_message>
<xml_diff>
--- a/inst/extdata/moxy_ramp_example.xlsx
+++ b/inst/extdata/moxy_ramp_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R-Projects\mNIRS\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3600E56-136A-4557-AABE-33BDA6460561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ECB7501-D92D-4AF7-90C1-36C328B8F7E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="29010" windowHeight="31785" xr2:uid="{ED07EABD-9B2D-42C5-B904-3B14C8E7B28A}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="31785" xr2:uid="{ED07EABD-9B2D-42C5-B904-3B14C8E7B28A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -7529,8 +7529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7B18608-BA4B-422A-BDE0-919FC8A5223C}">
   <dimension ref="A1:F2392"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1086" workbookViewId="0">
-      <selection activeCell="C1096" sqref="C1096"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>